<commit_message>
Added helmholtz coil power calculations and matlab file to simulate the design in FEMM
</commit_message>
<xml_diff>
--- a/Magnetics_testing/EM_coil_calculations/helmholtz_spec.xlsx
+++ b/Magnetics_testing/EM_coil_calculations/helmholtz_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="11240" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="11240" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="B2" s="2">
         <f>2*B5 + B1</f>
-        <v>3.6333333333333337</v>
+        <v>3.1550548832793028</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16">
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>6.4000000000000001E-2</v>
+        <v>6.4100000000000004E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" s="2">
         <f>SQRT(B4/0.9) * (B3/2)</f>
-        <v>1.0666666666666669</v>
+        <v>0.82752744163965142</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -506,7 +506,7 @@
       </c>
       <c r="B7" s="2">
         <f>B6*B13/(1.26*10^-6 * B4) * (4/5)^(-3/2)</f>
-        <v>15.354111613357931</v>
+        <v>22.221589368871737</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -515,7 +515,7 @@
       </c>
       <c r="B8" s="2">
         <f>2 * B13 * B4 / B14^2 * 1.7*10^-8</f>
-        <v>2.3747641896325455</v>
+        <v>1.2334379479013047</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -524,7 +524,7 @@
       </c>
       <c r="B9" s="2">
         <f>B7*B8</f>
-        <v>36.462394423023603</v>
+        <v>27.408951590246602</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -533,7 +533,7 @@
       </c>
       <c r="B10" s="2">
         <f>B7*B9</f>
-        <v>559.84767366138419</v>
+        <v>609.07046726974397</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -542,7 +542,7 @@
       </c>
       <c r="B11" s="2">
         <f>2*PI()*B13*B4</f>
-        <v>289.92711402429006</v>
+        <v>151.05731398305878</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -551,7 +551,7 @@
       </c>
       <c r="B13" s="2">
         <f>(B2/2)*0.0254</f>
-        <v>4.6143333333333335E-2</v>
+        <v>4.0069197017647142E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -560,13 +560,13 @@
       </c>
       <c r="B14" s="2">
         <f>(B3/2)*0.0254</f>
-        <v>8.1280000000000002E-4</v>
+        <v>8.1407000000000007E-4</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18">
         <f>2*PI()*B13</f>
-        <v>0.28992711402429006</v>
+        <v>0.25176218997176464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>